<commit_message>
need to complete verify api
</commit_message>
<xml_diff>
--- a/docs/SaltApiList_Updated_23_06.xlsx
+++ b/docs/SaltApiList_Updated_23_06.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\leoge\PhpstormProjects\sanextjs.loc\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB56FF9D-A37D-4C60-916B-E4924A0AE0BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D591D30F-0499-4F9D-A698-2DD0BCBEC152}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="16170" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="16080" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -7995,8 +7995,8 @@
   <dimension ref="A1:Z1000"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="40" zoomScaleNormal="40" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G32" sqref="G32"/>
+      <pane ySplit="1" topLeftCell="A59" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D36" sqref="D36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.7109375" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -9442,10 +9442,10 @@
       <c r="C36" s="29" t="s">
         <v>123</v>
       </c>
-      <c r="D36" s="10" t="s">
+      <c r="D36" s="27" t="s">
         <v>124</v>
       </c>
-      <c r="E36" s="10" t="s">
+      <c r="E36" s="27" t="s">
         <v>125</v>
       </c>
       <c r="F36" s="10" t="s">
@@ -9484,10 +9484,10 @@
       <c r="C37" s="29" t="s">
         <v>127</v>
       </c>
-      <c r="D37" s="10" t="s">
+      <c r="D37" s="27" t="s">
         <v>128</v>
       </c>
-      <c r="E37" s="10" t="s">
+      <c r="E37" s="27" t="s">
         <v>129</v>
       </c>
       <c r="F37" s="10" t="s">

</xml_diff>